<commit_message>
se agrega style al modal de comprar para que genere scroll cuando agregan muchos productos
se agrega style al modal de comprar para que genere scroll cuando agregan muchos productos
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/SPRINT 10.xlsx
+++ b/Analisis/SPRINTs/SPRINT 10.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C582A7-9976-413E-B01D-433E7CD8AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CB26D9-5238-4379-87B1-68071C81C689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1C0185E2-95A7-44C4-B2F2-7D0A36D029E1}"/>
   </bookViews>
@@ -239,15 +239,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,23 +747,23 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:R2"/>
+      <selection activeCell="K3" sqref="K3:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
       <c r="K1" s="3" t="s">
         <v>28</v>
       </c>
@@ -790,16 +790,16 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -820,16 +820,16 @@
       <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -851,14 +851,14 @@
       <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -880,14 +880,14 @@
       <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -908,14 +908,14 @@
       <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -936,14 +936,14 @@
       <c r="H7" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -964,14 +964,14 @@
       <c r="H8" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -992,14 +992,14 @@
       <c r="H9" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1020,14 +1020,14 @@
       <c r="H10" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1048,14 +1048,14 @@
       <c r="H11" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1237,19 +1237,19 @@
       <c r="H20" t="s">
         <v>0</v>
       </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -1285,57 +1285,63 @@
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
-      <c r="V25" s="6"/>
-      <c r="W25" s="6"/>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="6"/>
-      <c r="AA25" s="6"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
     </row>
     <row r="26" spans="1:27" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K26" s="7" t="s">
+      <c r="K26" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="6"/>
-      <c r="AA26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
     </row>
     <row r="27" spans="1:27" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K27" s="7" t="s">
+      <c r="K27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="K5:R5"/>
     <mergeCell ref="K20:W20"/>
     <mergeCell ref="K25:N25"/>
     <mergeCell ref="K26:N26"/>
@@ -1345,12 +1351,6 @@
     <mergeCell ref="K9:R9"/>
     <mergeCell ref="K10:R10"/>
     <mergeCell ref="K11:R11"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="K3:R3"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="K5:R5"/>
-    <mergeCell ref="K6:R6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>